<commit_message>
[테마] Zerif Lite 테마 설정 및 수정 방법 manual update
</commit_message>
<xml_diff>
--- a/Zerif Lite_Onsemi14 design Data.xlsx
+++ b/Zerif Lite_Onsemi14 design Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t>1. 사이드바 제거</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>부모 테마인 Zerif Lite의 page.php 수정 필요</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -32,19 +28,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2. Home의 Big title section의 background 이미지의 색 및 투명도 조절</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>차일드 style.css의 .header-content-wrap class 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3. Home의 Big title section의 text의 색 및 투명도 조절</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4. footer의 copyright 수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -81,6 +65,22 @@
   </si>
   <si>
     <t>Home의 두번째 content 설정 부분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 사이드바 제거 : page.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Home의 Big title section의 background 이미지의 색 및 투명도 조절 : style.css</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. Home의 Big title section의 text의 색 및 투명도 조절 : style.css</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. footer의 copyright 수정 : footer.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3667,8 +3667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C82"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W90" sqref="W90"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S72" sqref="S72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3680,42 +3680,42 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B81" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C82" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3733,8 +3733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="N217" sqref="N217"/>
+    <sheetView topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="T177" sqref="T177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3746,42 +3746,42 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P35" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J49" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B117" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C118" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="165" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B165" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="166" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C166" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>